<commit_message>
update on modeling. continue to optimization tmr...
</commit_message>
<xml_diff>
--- a/other/HSPICE.xlsx
+++ b/other/HSPICE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="14355" windowHeight="11055" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="14355" windowHeight="11055"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -189,8 +189,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.20235106279111173"/>
-          <c:y val="4.6994792317626967E-2"/>
-          <c:w val="0.77274752034551486"/>
+          <c:y val="4.6994792317626981E-2"/>
+          <c:w val="0.77274752034551508"/>
           <c:h val="0.75116010498687669"/>
         </c:manualLayout>
       </c:layout>
@@ -1226,11 +1226,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="64937984"/>
-        <c:axId val="64939904"/>
+        <c:axId val="95466240"/>
+        <c:axId val="95468544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64937984"/>
+        <c:axId val="95466240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1263,7 +1263,7 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.28396905529040822"/>
+              <c:x val="0.28396905529040828"/>
               <c:y val="0.90177761113194188"/>
             </c:manualLayout>
           </c:layout>
@@ -1271,12 +1271,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64939904"/>
+        <c:crossAx val="95468544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64939904"/>
+        <c:axId val="95468544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1302,7 +1302,7 @@
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64937984"/>
+        <c:crossAx val="95466240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1313,8 +1313,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.53805981035740358"/>
-          <c:y val="0.36946881639795043"/>
+          <c:x val="0.5380598103574038"/>
+          <c:y val="0.36946881639795059"/>
           <c:w val="0.44443471918307798"/>
           <c:h val="0.23989801274840644"/>
         </c:manualLayout>
@@ -1334,7 +1334,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2364,11 +2364,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="66312832"/>
-        <c:axId val="85988480"/>
+        <c:axId val="97990912"/>
+        <c:axId val="98013568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66312832"/>
+        <c:axId val="97990912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2402,12 +2402,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85988480"/>
+        <c:crossAx val="98013568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85988480"/>
+        <c:axId val="98013568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2434,7 +2434,7 @@
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66312832"/>
+        <c:crossAx val="97990912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2443,7 +2443,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2462,8 +2462,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.20235106279111173"/>
-          <c:y val="4.6994792317626988E-2"/>
-          <c:w val="0.7727475203455153"/>
+          <c:y val="4.6994792317626995E-2"/>
+          <c:w val="0.77274752034551553"/>
           <c:h val="0.75116010498687669"/>
         </c:manualLayout>
       </c:layout>
@@ -3499,11 +3499,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="97872128"/>
-        <c:axId val="97888512"/>
+        <c:axId val="100185984"/>
+        <c:axId val="100200448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97872128"/>
+        <c:axId val="100185984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3536,7 +3536,7 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.28396905529040833"/>
+              <c:x val="0.28396905529040839"/>
               <c:y val="0.90177761113194188"/>
             </c:manualLayout>
           </c:layout>
@@ -3544,12 +3544,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97888512"/>
+        <c:crossAx val="100200448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97888512"/>
+        <c:axId val="100200448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3584,7 +3584,7 @@
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97872128"/>
+        <c:crossAx val="100185984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3595,8 +3595,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.53805981035740391"/>
-          <c:y val="0.36946881639795076"/>
+          <c:x val="0.53805981035740402"/>
+          <c:y val="0.36946881639795093"/>
           <c:w val="0.44443471918307798"/>
           <c:h val="0.23989801274840644"/>
         </c:manualLayout>
@@ -3621,7 +3621,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3728,19 +3728,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ronm_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ronm" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ronm" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="negwrite" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="negwrite" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ronm_2" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ronm_2" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ronm_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4030,7 +4030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:N170"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
       <selection activeCell="M170" activeCellId="1" sqref="B92:B170 L92:M170"/>
     </sheetView>
   </sheetViews>
@@ -10065,7 +10065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>